<commit_message>
made changes to the data files
</commit_message>
<xml_diff>
--- a/data/describe/LessonTree.xlsx
+++ b/data/describe/LessonTree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\twelve-gpt-educational\data\describe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B995C2-B8C4-488F-9A0E-558B847EFC53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468E78DA-34AF-4DCB-8172-2CC5AE337949}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="90">
   <si>
     <t>step</t>
   </si>
@@ -69,103 +69,277 @@
     <t>printing 1 to 10</t>
   </si>
   <si>
+    <t>1.2.1</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>assistant</t>
+  </si>
+  <si>
+    <t>1.1.</t>
+  </si>
+  <si>
+    <t>Tell the user you are really happy they know so much. Then ask them to write a loop which prints out the numbers 1 to 10.</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>OK let’s help the user learn about variables first. Ask the user if they can you define a variable for you?</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Tell the user that they are right, thats exactly what they are. Now the use  to write the syntax of a for loop?</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>For loops are used to achieve repetition in programming. Can you tell me why repetition is important</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>1.1.1.1</t>
+  </si>
+  <si>
+    <t>It reduces the amount of code I will end up writing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tell the user that is right and ask them to write for you the syntax of a for loop
+</t>
+  </si>
+  <si>
+    <t>1.1.1.2</t>
+  </si>
+  <si>
+    <t>for(initialization; condition; increment)</t>
+  </si>
+  <si>
+    <t>Check if what he user has written is correct. If its correct ask the user to explain what each componenet of the for loop means</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
+  </si>
+  <si>
+    <t>I don't know how to write the syntax of a for loop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tell the user that is okay and give the user the syntax of a for loop with an explanation of what each component is then ask the user if they can write the code to display numbers 1 to 10 using the syntax provided
+</t>
+  </si>
+  <si>
+    <t>int i=5;</t>
+  </si>
+  <si>
+    <t>Check the user code, if it is correct tell the user the relationship between variables and loops.</t>
+  </si>
+  <si>
+    <t>variables</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>Variables help in tracking the number of iterations</t>
+  </si>
+  <si>
+    <t>Tell the user they are rigth, then tell them what for loops are and how variables are used in the for loop.</t>
+  </si>
+  <si>
+    <t>I think I missed  I used the ", " instead of the ";"</t>
+  </si>
+  <si>
+    <t>Can you identify the problem expecially in the defination of the loop?</t>
+  </si>
+  <si>
+    <t>1.2.1.1</t>
+  </si>
+  <si>
+    <t>Right, now correct your code to provide the right solution to the problem</t>
+  </si>
+  <si>
+    <t>I don't know how to define a loop</t>
+  </si>
+  <si>
+    <t>There seems to be a problem with your loop defination. Relook at your code and tell me if you can correct it</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>1.2.2.1</t>
+  </si>
+  <si>
+    <t>A loop has a header and a body</t>
+  </si>
+  <si>
+    <t>Tell me the difference components that entail loop defination</t>
+  </si>
+  <si>
+    <t>1.2.2.3</t>
+  </si>
+  <si>
+    <t>The start of the interation, the condition to end the loop and the increment of the iterating variable</t>
+  </si>
+  <si>
+    <t>What do you need to define in the header of the for loop</t>
+  </si>
+  <si>
+    <t>1.2.2.4</t>
+  </si>
+  <si>
+    <t>Could you write for me the syntax of a for loop in c</t>
+  </si>
+  <si>
+    <t>1.2.2.5</t>
+  </si>
+  <si>
+    <t>There is a missing start and the increment</t>
+  </si>
+  <si>
+    <t>Could you now look at the head of the solution provided and tell me  if all the component of the loop head are included</t>
+  </si>
+  <si>
+    <t>1.2.2.6</t>
+  </si>
+  <si>
     <t>#include&lt;stdio.h&gt;
 int main()
 {
     int i;
-    for(i=1,i&lt;=10,i++)
+    for(i=0;i&lt;=10;i++)
     {
         printf("%d ",i);
     }
 }</t>
   </si>
   <si>
-    <t>1.2.1</t>
-  </si>
-  <si>
-    <t>The syntax for the for loop is
-for(intialization;condition;increment)
+    <t>Perfect, now can you provide me with the corrected code</t>
+  </si>
+  <si>
+    <t>I think it is perfect</t>
+  </si>
+  <si>
+    <t>Your printf statement seems to have a problem, can you indetify what the problem is</t>
+  </si>
+  <si>
+    <t>Integer display</t>
+  </si>
+  <si>
+    <t>1.2.3.1</t>
+  </si>
+  <si>
+    <t>I use the access specify %d and then provide the integer value</t>
+  </si>
+  <si>
+    <t>How do you display a integer using the printf statement</t>
+  </si>
+  <si>
+    <t>1.2.3.2</t>
+  </si>
+  <si>
+    <t>Can you correct your code now to display the integers</t>
+  </si>
+  <si>
+    <t>#include &lt;stdio.h&gt;
+int main()
 {
-      //what is to be reapeted
+    int i;
+    for(i=1;i&lt;20;i++)
+    {
+        if(i%2==0)
+        {
+            printf("%d ", i);
+        }
+    }
 }</t>
   </si>
   <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>assistant</t>
-  </si>
-  <si>
-    <t>int a =5</t>
-  </si>
-  <si>
-    <t>variable defination</t>
-  </si>
-  <si>
-    <t>I know what loops do</t>
-  </si>
-  <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>1.1.1.</t>
-  </si>
-  <si>
-    <t>1.1.</t>
-  </si>
-  <si>
-    <t>1.2.</t>
-  </si>
-  <si>
-    <t>1.1.2.</t>
-  </si>
-  <si>
-    <t>1.3.</t>
-  </si>
-  <si>
-    <t>Your code is correct, can you now write a loop that only displays number even numbers</t>
-  </si>
-  <si>
-    <t>1.4.</t>
-  </si>
-  <si>
-    <t>1.1.1.1.</t>
-  </si>
-  <si>
-    <t>1.1.1.2.</t>
-  </si>
-  <si>
-    <t>Good attempt, You missed a semi colon at the end of the statement, all statements in C have to end with a semi colon. Correct your code and submit again</t>
-  </si>
-  <si>
-    <t>Great, can you tell me what loops do?[1.1.1.]</t>
-  </si>
-  <si>
-    <t>I am glad you know how to write a loop. Can you write a loop to displays numbers 1 to 10 [1.3.]</t>
-  </si>
-  <si>
-    <t>OK let’s lets start by learning about variables, one of the building blocks of loops. Can you define a variable that will store number 5 [1.2.]</t>
-  </si>
-  <si>
-    <t>That is correct, thats exactly what they are. Write for me the syntax of a for loop. [1.1.2.]</t>
-  </si>
-  <si>
-    <t>That is correct,how do you write the initialization part of the loop if the loop was to start from 1?</t>
-  </si>
-  <si>
-    <t>i=1</t>
-  </si>
-  <si>
-    <t>That is correct, now write the condition part of the loop for a loop that will have to display numbers from 1 to 10</t>
-  </si>
-  <si>
-    <t>Your code seems to have a problem at the loop defination, can you check to see if you can spot the error</t>
-  </si>
-  <si>
-    <t>I cannot see the error</t>
-  </si>
-  <si>
-    <t>Okay, what sybols do you use to separate statements in the loop</t>
+    <t>Write a program to display only even numbers between 1 and 20</t>
+  </si>
+  <si>
+    <t>Loops and if statements</t>
+  </si>
+  <si>
+    <t>#include &lt;stdio.h&gt;
+int main()
+{
+    int i;
+    for(i=1;i&lt;20;i++)
+    {
+        if(i=="even")
+        {
+            printf("%d ", i);
+        }
+    }
+}</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>A number is even if when you divide by 2 there is no reminder</t>
+  </si>
+  <si>
+    <t>You seem to have a problem with your if statement. How do you know a number is even</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>You use the modulas operator</t>
+  </si>
+  <si>
+    <t>How do you check for the reminder of dividing two number</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>Can you now use the modulas operator to correct your code</t>
+  </si>
+  <si>
+    <t>Use the for loop to calculate the sum of numbers between 1 and 10</t>
+  </si>
+  <si>
+    <t>Loops and aggregation</t>
+  </si>
+  <si>
+    <t>#include &lt;stdio.h&gt;
+int main()
+{
+    int i;
+    int sum;
+    for(i=1;i&lt;10;i++)
+    {
+        sum+=i;
+    }
+    printf("%d",sum);
+}</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>I cant seem to see the issue with my code</t>
+  </si>
+  <si>
+    <t>There seems to be an issue with your sum, can you identify it?</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>The variable sum needs to be intialize. Which number should it be initialized too</t>
+  </si>
+  <si>
+    <t>Check the code to see if it does write out the numbers 1 to 10. If you think it does then congratulate them on their great coding, and ask them to write a loop that will only display even numbers between 1 to 10. Now ask them to copy the code into code runner and check it. Otherwise tell them where you think the error is in their code and ask them to try again.</t>
   </si>
 </sst>
 </file>
@@ -324,7 +498,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -358,14 +532,20 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1497,10 +1677,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1510,16 +1690,16 @@
     <col min="3" max="3" width="6.6328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.453125" style="1" customWidth="1"/>
-    <col min="6" max="11" width="8.36328125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.36328125" style="1"/>
+    <col min="6" max="12" width="8.36328125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.36328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" customHeight="1">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1531,183 +1711,533 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32.25" customHeight="1">
+    <row r="2" spans="1:6" ht="32.25" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="20" customHeight="1">
+        <v>18</v>
+      </c>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="20" customHeight="1">
+        <v>20</v>
+      </c>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" ht="20" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
       <c r="D4" s="9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="20" customHeight="1">
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" ht="20" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="20" customHeight="1">
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" ht="20" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="A7" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="20" customHeight="1">
-      <c r="A7" s="7" t="s">
+      <c r="B7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" ht="80" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="80" customHeight="1">
-      <c r="A8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="128" customHeight="1">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" ht="128" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>26</v>
+        <v>89</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="128" customHeight="1">
+        <v>16</v>
+      </c>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" ht="128" customHeight="1">
       <c r="A10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="19.899999999999999" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="D12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A16" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A19" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="13">
+        <v>2</v>
+      </c>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="19.899999999999999" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="D20" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A21" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="13">
+        <v>2</v>
+      </c>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A23" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="13">
+        <v>2</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="13">
+        <v>3</v>
+      </c>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A24" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="13">
+        <v>2</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A25" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A26" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A27" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="13">
+        <v>3</v>
+      </c>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A28" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="13">
+        <v>3</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="13">
+        <v>4</v>
+      </c>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A29" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="13">
+        <v>3</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A30" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" spans="1:6" ht="19.899999999999999" customHeight="1">
+      <c r="A31" s="15"/>
+      <c r="B31" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Provided the relevant information that was missing
</commit_message>
<xml_diff>
--- a/data/describe/LessonTree.xlsx
+++ b/data/describe/LessonTree.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\twelve-gpt-educational\data\describe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83889133-7007-407E-B83C-994AD997B00F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EB7F81-5A16-4ABE-880D-70A98907EDF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,19 +229,21 @@
     <t>Check the user code, if it is correct, congragulate the user and ask them a more complex task</t>
   </si>
   <si>
-    <t>loops and a+A10rrays</t>
-  </si>
-  <si>
     <t>1.</t>
   </si>
   <si>
-    <t>That is great. Write a  for loop that will display numbers 1 to 10.</t>
-  </si>
-  <si>
-    <t>Welcome to interactive teaching bot, the bot is meant for teaching C programming. Start by respoding on what you know about for loops.</t>
-  </si>
-  <si>
-    <t>beginning</t>
+    <t>I know a little bit of the for loop</t>
+  </si>
+  <si>
+    <t>Tell the user you are happy they know how to write a for loop. Ask the user to write a  for loop that will display numbers 1 to 10.</t>
+  </si>
+  <si>
+    <t>Tell the user it is great they know about for loops and ask the user to write the syntax of the for loop</t>
+  </si>
+  <si>
+    <t>int numbers[]=[45,67,77,56,78];
+for(i=0;i&lt;5;i++)
+{printf("%d",i)}</t>
   </si>
 </sst>
 </file>
@@ -1619,8 +1621,8 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1653,13 +1655,13 @@
     </row>
     <row r="2" spans="1:6" ht="20.25" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
@@ -1672,7 +1674,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>3</v>
@@ -1690,7 +1692,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>3</v>
@@ -1708,7 +1710,7 @@
         <v>29</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>6</v>
@@ -1810,7 +1812,7 @@
     </row>
     <row r="11" spans="1:6" ht="128" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
saving the local recent changes
</commit_message>
<xml_diff>
--- a/data/describe/LessonTree.xlsx
+++ b/data/describe/LessonTree.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\twelve-gpt-educational\data\describe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D802B0-E6AF-4440-B7BE-8EA191E4B016}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716A0CD4-809F-402A-8B5A-260A03A53960}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1792,8 +1792,8 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>

</xml_diff>

<commit_message>
Added saving the chat conversation to github
</commit_message>
<xml_diff>
--- a/data/describe/LessonTree.xlsx
+++ b/data/describe/LessonTree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\twelve-gpt-educational\data\describe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716A0CD4-809F-402A-8B5A-260A03A53960}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4FC9BD-37F3-4326-BF56-21857B678890}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,56 +259,56 @@
     <t>Tell the user they are right and ask the use to write code to set up a variable called number,  initialising it with the value 5 using the C programming language.</t>
   </si>
   <si>
-    <t>Check the users code very carefully. It should correctly define a variable and set it to a value to 5 according to the C programming lanagauge.  If the user answer is correct, start to explain the relations between variables and the for loop.In particular how we initialise a variable in a loop in C. Write the initialization part of the for loop as follows;_x000B__x000B_for(int i=0;{end condition};{increment})
+    <t>for(int i=0;i&lt;=10;i++)</t>
+  </si>
+  <si>
+    <t>Check the user answer carefully. It should correctily have a condition that will loop until 10 and increment the loop variable by 1. If the user answer is correct, ask the user to know create the whole program that will display values from 1 to 10.
+If the user's answer is not correct, tell the user where the error is without providing the solution and ask them to try again.</t>
+  </si>
+  <si>
+    <t>1.3.1.1.1</t>
+  </si>
+  <si>
+    <t>1.2.1</t>
+  </si>
+  <si>
+    <t>1.2.1.1.1., 1.2.1.1.2.</t>
+  </si>
+  <si>
+    <t>1.2.1.1.2.</t>
+  </si>
+  <si>
+    <t>1.2.1.1.2.1</t>
+  </si>
+  <si>
+    <t>1.2.1.1.2.1.</t>
+  </si>
+  <si>
+    <t>1.2.1.2.2.1</t>
+  </si>
+  <si>
+    <t>1.1.1.1</t>
+  </si>
+  <si>
+    <t>Tell the user, that is okay, then ask the user to tell you what a loop is in general terms. In particular ask the user what they understand by the term loop as used in everyday life.</t>
+  </si>
+  <si>
+    <t>Loops generally is something that happens repeatedly</t>
+  </si>
+  <si>
+    <t>Tell the user they are right, then explain to the user how the concept of repeating applies to loops in programming. Tell the user, that before you explain to them about for loops, you would like them to understand about variables. Ask the user what variables are?</t>
+  </si>
+  <si>
+    <t>1.1.2.1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tell the user that is okay and give the user the syntax of a for loop with an explanation of what each component is. Give the user a simple example that follows the syntax,  then ask the user if they can follow the syntax to write the code to display numbers 1 to 10 using the C programming language.
+</t>
+  </si>
+  <si>
+    <t>Check if the user answer is correct per the question. Check the users code very carefully. It should correctly define a variable and set it to a value to 5 according to the C programming lanagauge.  If the user answer is correct, start to explain the relations between variables and the for loop.In particular how we initialise a variable in a loop in C. Write the initialization part of the for loop as follows;_x000B__x000B_for(int i=0;{end condition};{increment})
 And tell the user that this initialises the loop variable to 0, the loop will  loop over until the loop variable value reaches satisfies the loop condition. Now ask them to write an end condition and an increment so that the variable should continue to increase until it is 10.
 If the user has an error in their code and it is not valid C syntax, tell the user what is wrong, but don’t give the entire correct answer. Then ask them to try again.</t>
-  </si>
-  <si>
-    <t>for(int i=0;i&lt;=10;i++)</t>
-  </si>
-  <si>
-    <t>Check the user answer carefully. It should correctily have a condition that will loop until 10 and increment the loop variable by 1. If the user answer is correct, ask the user to know create the whole program that will display values from 1 to 10.
-If the user's answer is not correct, tell the user where the error is without providing the solution and ask them to try again.</t>
-  </si>
-  <si>
-    <t>1.3.1.1.1</t>
-  </si>
-  <si>
-    <t>1.2.1</t>
-  </si>
-  <si>
-    <t>1.2.1.1.1., 1.2.1.1.2.</t>
-  </si>
-  <si>
-    <t>1.2.1.1.2.</t>
-  </si>
-  <si>
-    <t>1.2.1.1.2.1</t>
-  </si>
-  <si>
-    <t>1.2.1.1.2.1.</t>
-  </si>
-  <si>
-    <t>1.2.1.2.2.1</t>
-  </si>
-  <si>
-    <t>1.1.1.1</t>
-  </si>
-  <si>
-    <t>Tell the user, that is okay, then ask the user to tell you what a loop is in general terms. In particular ask the user what they understand by the term loop as used in everyday life.</t>
-  </si>
-  <si>
-    <t>Loops generally is something that happens repeatedly</t>
-  </si>
-  <si>
-    <t>Tell the user they are right, then explain to the user how the concept of repeating applies to loops in programming. Tell the user, that before you explain to them about for loops, you would like them to understand about variables. Ask the user what variables are?</t>
-  </si>
-  <si>
-    <t>1.1.2.1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tell the user that is okay and give the user the syntax of a for loop with an explanation of what each component is. Give the user a simple example that follows the syntax,  then ask the user if they can follow the syntax to write the code to display numbers 1 to 10 using the C programming language.
-</t>
   </si>
 </sst>
 </file>
@@ -1792,8 +1792,8 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1803,8 +1803,8 @@
     <col min="3" max="3" width="6.6328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.6328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
-    <col min="6" max="12" width="8.36328125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.36328125" style="1"/>
+    <col min="6" max="13" width="8.36328125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.36328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" customHeight="1">
@@ -1923,7 +1923,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="40.9" customHeight="1">
@@ -1931,7 +1931,7 @@
         <v>44</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>36</v>
@@ -1940,15 +1940,15 @@
         <v>11</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="40.9" customHeight="1">
       <c r="A9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>59</v>
@@ -1968,7 +1968,7 @@
         <v>56</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>11</v>
@@ -1982,7 +1982,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>13</v>
@@ -2025,7 +2025,7 @@
         <v>45</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="128" customHeight="1">
@@ -2036,13 +2036,13 @@
         <v>31</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="128" customHeight="1">
@@ -2070,7 +2070,7 @@
         <v>47</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>19</v>
@@ -2110,7 +2110,7 @@
         <v>19</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="128" customHeight="1">
@@ -2121,7 +2121,7 @@
         <v>53</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>19</v>
@@ -2133,7 +2133,7 @@
         <v>26</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>58</v>
@@ -2142,24 +2142,24 @@
         <v>28</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="200.9" customHeight="1">
       <c r="A21" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="C21" s="27" t="s">
         <v>63</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>64</v>
       </c>
       <c r="D21" s="28" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>